<commit_message>
Updating to how traumarl was released
</commit_message>
<xml_diff>
--- a/RogueBasin/docs/traumarl_combat.xlsx
+++ b/RogueBasin/docs/traumarl_combat.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="97">
   <si>
     <t>TraumaRL combat</t>
   </si>
@@ -39,9 +39,6 @@
     <t>Laser</t>
   </si>
   <si>
-    <t>Blade</t>
-  </si>
-  <si>
     <t>Fists</t>
   </si>
   <si>
@@ -270,9 +267,6 @@
     <t>These are good, intro turret</t>
   </si>
   <si>
-    <t>A bit nothingy at the moment</t>
-  </si>
-  <si>
     <t>OK / Good</t>
   </si>
   <si>
@@ -304,13 +298,22 @@
   </si>
   <si>
     <t>Drop chance used</t>
+  </si>
+  <si>
+    <t>Ultra swarmer bot</t>
+  </si>
+  <si>
+    <t>A bit nothingy at the moment (100 damage on higher levels)</t>
+  </si>
+  <si>
+    <t>Vibroknife</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -320,6 +323,14 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -347,10 +358,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -645,10 +657,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:T81"/>
+  <dimension ref="A1:T82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="T55" sqref="T55"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -667,22 +679,22 @@
     </row>
     <row r="3" spans="1:15">
       <c r="D3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" t="s">
         <v>11</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>12</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>13</v>
       </c>
-      <c r="H3" t="s">
-        <v>14</v>
-      </c>
       <c r="O3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:15">
@@ -699,12 +711,12 @@
         <v>4</v>
       </c>
       <c r="O5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:15">
       <c r="O6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:15">
@@ -715,7 +727,7 @@
         <v>50</v>
       </c>
       <c r="O7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:15">
@@ -742,18 +754,18 @@
         <v>400</v>
       </c>
       <c r="O8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:15">
       <c r="A10" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B10">
         <v>20</v>
       </c>
       <c r="D10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E10">
         <f>E$8/$B10</f>
@@ -816,16 +828,16 @@
     </row>
     <row r="14" spans="1:15">
       <c r="D14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E14" t="s">
         <v>11</v>
       </c>
-      <c r="E14" t="s">
+      <c r="F14" t="s">
         <v>12</v>
       </c>
-      <c r="F14" t="s">
+      <c r="G14" t="s">
         <v>13</v>
-      </c>
-      <c r="G14" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:15">
@@ -833,7 +845,7 @@
         <v>3</v>
       </c>
       <c r="C15" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D15">
         <v>1</v>
@@ -850,7 +862,7 @@
     </row>
     <row r="16" spans="1:15">
       <c r="C16" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D16">
         <v>1</v>
@@ -867,12 +879,12 @@
     </row>
     <row r="17" spans="1:12">
       <c r="A17" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="18" spans="1:12">
       <c r="A18" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B18">
         <v>10</v>
@@ -896,7 +908,7 @@
     </row>
     <row r="19" spans="1:12">
       <c r="A19" t="s">
-        <v>7</v>
+        <v>96</v>
       </c>
       <c r="B19">
         <v>30</v>
@@ -918,130 +930,130 @@
         <v>300</v>
       </c>
     </row>
-    <row r="20" spans="1:12">
-      <c r="A20" t="s">
-        <v>27</v>
-      </c>
-      <c r="B20">
+    <row r="20" spans="1:12" s="3" customFormat="1">
+      <c r="A20" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B20" s="3">
         <v>50</v>
       </c>
-      <c r="D20">
+      <c r="D20" s="3">
         <f t="shared" si="4"/>
         <v>50</v>
       </c>
-      <c r="E20">
+      <c r="E20" s="3">
         <f t="shared" si="5"/>
         <v>150</v>
       </c>
-      <c r="F20">
+      <c r="F20" s="3">
         <f t="shared" si="5"/>
         <v>300</v>
       </c>
-      <c r="G20">
+      <c r="G20" s="3">
         <f t="shared" si="5"/>
         <v>500</v>
       </c>
     </row>
-    <row r="21" spans="1:12">
-      <c r="A21" t="s">
-        <v>17</v>
-      </c>
-      <c r="B21">
+    <row r="21" spans="1:12" s="3" customFormat="1">
+      <c r="A21" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B21" s="3">
         <v>100</v>
       </c>
-      <c r="D21">
+      <c r="D21" s="3">
         <f t="shared" si="4"/>
         <v>100</v>
       </c>
-      <c r="E21">
+      <c r="E21" s="3">
         <f t="shared" si="5"/>
         <v>300</v>
       </c>
-      <c r="F21">
+      <c r="F21" s="3">
         <f t="shared" si="5"/>
         <v>600</v>
       </c>
-      <c r="G21">
+      <c r="G21" s="3">
         <f t="shared" si="5"/>
         <v>1000</v>
       </c>
     </row>
-    <row r="22" spans="1:12">
-      <c r="A22" t="s">
-        <v>18</v>
-      </c>
-      <c r="B22">
+    <row r="22" spans="1:12" s="3" customFormat="1">
+      <c r="A22" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B22" s="3">
         <v>20</v>
       </c>
-      <c r="D22">
+      <c r="D22" s="3">
         <f t="shared" si="4"/>
         <v>20</v>
       </c>
-      <c r="E22">
+      <c r="E22" s="3">
         <f t="shared" si="5"/>
         <v>60</v>
       </c>
-      <c r="F22">
+      <c r="F22" s="3">
         <f t="shared" si="5"/>
         <v>120</v>
       </c>
-      <c r="G22">
+      <c r="G22" s="3">
         <f t="shared" si="5"/>
         <v>200</v>
       </c>
     </row>
-    <row r="23" spans="1:12">
-      <c r="A23" t="s">
-        <v>19</v>
-      </c>
-      <c r="B23">
+    <row r="23" spans="1:12" s="3" customFormat="1">
+      <c r="A23" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B23" s="3">
         <v>20</v>
       </c>
-      <c r="D23">
+      <c r="D23" s="3">
         <f t="shared" si="4"/>
         <v>20</v>
       </c>
-      <c r="E23">
+      <c r="E23" s="3">
         <f t="shared" si="5"/>
         <v>60</v>
       </c>
-      <c r="F23">
+      <c r="F23" s="3">
         <f t="shared" si="5"/>
         <v>120</v>
       </c>
-      <c r="G23">
+      <c r="G23" s="3">
         <f t="shared" si="5"/>
         <v>200</v>
       </c>
     </row>
     <row r="25" spans="1:12">
       <c r="D25" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E25">
         <v>0.45</v>
       </c>
       <c r="F25" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="26" spans="1:12">
       <c r="D26" t="s">
+        <v>10</v>
+      </c>
+      <c r="E26" t="s">
         <v>11</v>
       </c>
-      <c r="E26" t="s">
+      <c r="F26" t="s">
         <v>12</v>
       </c>
-      <c r="F26" t="s">
-        <v>13</v>
-      </c>
       <c r="G26" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="27" spans="1:12">
       <c r="C27" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D27">
         <v>0</v>
@@ -1058,7 +1070,7 @@
     </row>
     <row r="28" spans="1:12">
       <c r="B28" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C28">
         <v>1</v>
@@ -1121,13 +1133,13 @@
     </row>
     <row r="31" spans="1:12">
       <c r="A31" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D31" t="s">
+        <v>30</v>
+      </c>
+      <c r="I31" t="s">
         <v>31</v>
-      </c>
-      <c r="I31" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="32" spans="1:12">
@@ -1172,7 +1184,7 @@
     </row>
     <row r="33" spans="1:14">
       <c r="A33" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B33">
         <v>40</v>
@@ -1212,7 +1224,7 @@
     </row>
     <row r="34" spans="1:14">
       <c r="A34" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B34">
         <v>60</v>
@@ -1292,42 +1304,42 @@
     </row>
     <row r="36" spans="1:14">
       <c r="A36" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B36">
-        <v>200</v>
+        <v>150</v>
       </c>
       <c r="D36">
         <f t="shared" si="7"/>
-        <v>320</v>
+        <v>240</v>
       </c>
       <c r="E36">
         <f t="shared" si="10"/>
-        <v>470</v>
+        <v>352.5</v>
       </c>
       <c r="F36">
         <f t="shared" si="10"/>
-        <v>740</v>
+        <v>555</v>
       </c>
       <c r="G36">
         <f t="shared" si="10"/>
-        <v>1010.0000000000001</v>
+        <v>757.50000000000011</v>
       </c>
       <c r="I36">
         <f t="shared" si="15"/>
-        <v>240</v>
+        <v>180</v>
       </c>
       <c r="J36">
         <f t="shared" si="9"/>
-        <v>290</v>
+        <v>217.5</v>
       </c>
       <c r="K36">
         <f t="shared" si="9"/>
-        <v>380</v>
+        <v>285</v>
       </c>
       <c r="L36">
         <f t="shared" si="9"/>
-        <v>470</v>
+        <v>352.5</v>
       </c>
     </row>
     <row r="37" spans="1:14">
@@ -1372,7 +1384,7 @@
     </row>
     <row r="38" spans="1:14">
       <c r="A38" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B38">
         <v>150</v>
@@ -1412,57 +1424,57 @@
     </row>
     <row r="40" spans="1:14">
       <c r="A40" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="41" spans="1:14">
       <c r="A41" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B41">
-        <v>100</v>
+        <v>50</v>
       </c>
     </row>
     <row r="42" spans="1:14">
       <c r="A42" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B42">
-        <v>100</v>
+        <v>50</v>
       </c>
     </row>
     <row r="44" spans="1:14">
       <c r="A44" t="s">
+        <v>27</v>
+      </c>
+      <c r="B44" t="s">
         <v>28</v>
-      </c>
-      <c r="B44" t="s">
-        <v>29</v>
       </c>
       <c r="C44">
         <v>30</v>
       </c>
       <c r="E44" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F44">
         <v>100</v>
       </c>
       <c r="H44" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="45" spans="1:14">
       <c r="A45" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B45" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C45">
         <v>100</v>
       </c>
       <c r="E45" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F45">
         <v>100</v>
@@ -1470,44 +1482,44 @@
     </row>
     <row r="48" spans="1:14">
       <c r="A48" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="N48" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="49" spans="1:20">
       <c r="B49" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C49" t="s">
         <v>3</v>
       </c>
       <c r="D49" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G49" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="N49" t="s">
         <v>4</v>
       </c>
       <c r="O49" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="P49" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="R49" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="T49" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="50" spans="1:20">
       <c r="A50" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B50">
         <v>20</v>
@@ -1516,7 +1528,7 @@
         <v>10</v>
       </c>
       <c r="D50" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="N50">
         <f>CEILING(B50/$B$32,1)</f>
@@ -1540,7 +1552,7 @@
     </row>
     <row r="51" spans="1:20">
       <c r="A51" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B51">
         <v>20</v>
@@ -1549,25 +1561,25 @@
         <v>10</v>
       </c>
       <c r="D51" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G51" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="N51">
-        <f t="shared" ref="N51:N66" si="16">CEILING(B51/$B$32,1)</f>
+        <f t="shared" ref="N51:N67" si="16">CEILING(B51/$B$32,1)</f>
         <v>1</v>
       </c>
       <c r="O51">
-        <f t="shared" ref="O51:O66" si="17">CEILING(B51/$B$33,1)</f>
+        <f t="shared" ref="O51:O67" si="17">CEILING(B51/$B$33,1)</f>
         <v>1</v>
       </c>
       <c r="P51">
-        <f t="shared" ref="P51:P66" si="18">CEILING(B51/$B$34,1)</f>
+        <f t="shared" ref="P51:P67" si="18">CEILING(B51/$B$34,1)</f>
         <v>1</v>
       </c>
       <c r="R51">
-        <f t="shared" ref="R51:R70" si="19">P51*10</f>
+        <f t="shared" ref="R51:R71" si="19">P51*10</f>
         <v>10</v>
       </c>
       <c r="T51">
@@ -1576,7 +1588,7 @@
     </row>
     <row r="52" spans="1:20">
       <c r="A52" t="s">
-        <v>77</v>
+        <v>94</v>
       </c>
       <c r="B52">
         <v>40</v>
@@ -1585,46 +1597,24 @@
         <v>10</v>
       </c>
       <c r="D52" t="s">
-        <v>78</v>
-      </c>
-      <c r="G52" t="s">
-        <v>81</v>
-      </c>
-      <c r="N52">
-        <f t="shared" si="16"/>
-        <v>2</v>
-      </c>
-      <c r="O52">
-        <f t="shared" si="17"/>
-        <v>1</v>
-      </c>
-      <c r="P52">
-        <f t="shared" si="18"/>
-        <v>1</v>
-      </c>
-      <c r="R52">
-        <f t="shared" si="19"/>
-        <v>10</v>
-      </c>
-      <c r="T52">
-        <v>10</v>
+        <v>43</v>
       </c>
     </row>
     <row r="53" spans="1:20">
       <c r="A53" t="s">
-        <v>45</v>
+        <v>76</v>
       </c>
       <c r="B53">
         <v>40</v>
       </c>
       <c r="C53">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D53" t="s">
-        <v>50</v>
+        <v>77</v>
       </c>
       <c r="G53" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="N53">
         <f t="shared" si="16"/>
@@ -1648,127 +1638,127 @@
     </row>
     <row r="54" spans="1:20">
       <c r="A54" t="s">
-        <v>60</v>
+        <v>44</v>
       </c>
       <c r="B54">
-        <v>200</v>
+        <v>40</v>
       </c>
       <c r="C54">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="D54" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G54" t="s">
         <v>82</v>
       </c>
       <c r="N54">
         <f t="shared" si="16"/>
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="O54">
         <f t="shared" si="17"/>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="P54">
         <f t="shared" si="18"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="R54">
         <f t="shared" si="19"/>
+        <v>10</v>
+      </c>
+      <c r="T54">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="55" spans="1:20">
+      <c r="A55" t="s">
+        <v>59</v>
+      </c>
+      <c r="B55">
+        <v>200</v>
+      </c>
+      <c r="C55">
+        <v>30</v>
+      </c>
+      <c r="D55" t="s">
+        <v>49</v>
+      </c>
+      <c r="G55" t="s">
+        <v>81</v>
+      </c>
+      <c r="N55">
+        <f t="shared" si="16"/>
+        <v>10</v>
+      </c>
+      <c r="O55">
+        <f t="shared" si="17"/>
+        <v>5</v>
+      </c>
+      <c r="P55">
+        <f t="shared" si="18"/>
+        <v>4</v>
+      </c>
+      <c r="R55">
+        <f t="shared" si="19"/>
         <v>40</v>
       </c>
-      <c r="T54">
+      <c r="T55">
         <v>30</v>
       </c>
     </row>
-    <row r="56" spans="1:20">
-      <c r="A56" t="s">
+    <row r="57" spans="1:20">
+      <c r="A57" t="s">
+        <v>45</v>
+      </c>
+      <c r="B57">
+        <v>20</v>
+      </c>
+      <c r="C57">
+        <v>50</v>
+      </c>
+      <c r="D57" t="s">
         <v>46</v>
       </c>
-      <c r="B56">
-        <v>20</v>
-      </c>
-      <c r="C56">
-        <v>50</v>
-      </c>
-      <c r="D56" t="s">
-        <v>47</v>
-      </c>
-      <c r="G56" t="s">
-        <v>84</v>
-      </c>
-      <c r="N56">
+      <c r="G57" t="s">
+        <v>95</v>
+      </c>
+      <c r="N57">
         <f t="shared" si="16"/>
         <v>1</v>
       </c>
-      <c r="O56">
+      <c r="O57">
         <f t="shared" si="17"/>
         <v>1</v>
       </c>
-      <c r="P56">
+      <c r="P57">
         <f t="shared" si="18"/>
         <v>1</v>
       </c>
-      <c r="R56">
+      <c r="R57">
         <f t="shared" si="19"/>
         <v>10</v>
       </c>
-      <c r="T56">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="58" spans="1:20">
-      <c r="A58" t="s">
-        <v>70</v>
-      </c>
-      <c r="B58">
-        <v>10</v>
-      </c>
-      <c r="C58">
-        <v>0</v>
-      </c>
-      <c r="D58" t="s">
-        <v>71</v>
-      </c>
-      <c r="G58" t="s">
-        <v>85</v>
-      </c>
-      <c r="N58">
-        <f t="shared" si="16"/>
-        <v>1</v>
-      </c>
-      <c r="O58">
-        <f t="shared" si="17"/>
-        <v>1</v>
-      </c>
-      <c r="P58">
-        <f t="shared" si="18"/>
-        <v>1</v>
-      </c>
-      <c r="R58">
-        <f t="shared" si="19"/>
-        <v>10</v>
-      </c>
-      <c r="T58">
+      <c r="T57">
         <v>0</v>
       </c>
     </row>
     <row r="59" spans="1:20">
       <c r="A59" t="s">
-        <v>61</v>
+        <v>69</v>
       </c>
       <c r="B59">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="C59">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="D59" t="s">
-        <v>47</v>
+        <v>70</v>
       </c>
       <c r="G59" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="N59">
         <f t="shared" si="16"/>
@@ -1790,58 +1780,61 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:20">
-      <c r="A61" t="s">
-        <v>49</v>
-      </c>
-      <c r="B61">
+    <row r="60" spans="1:20">
+      <c r="A60" t="s">
+        <v>60</v>
+      </c>
+      <c r="B60">
         <v>20</v>
       </c>
-      <c r="C61">
-        <v>10</v>
-      </c>
-      <c r="D61" t="s">
-        <v>51</v>
-      </c>
-      <c r="G61" t="s">
-        <v>88</v>
-      </c>
-      <c r="N61">
+      <c r="C60">
+        <v>50</v>
+      </c>
+      <c r="D60" t="s">
+        <v>46</v>
+      </c>
+      <c r="G60" t="s">
+        <v>84</v>
+      </c>
+      <c r="N60">
         <f t="shared" si="16"/>
         <v>1</v>
       </c>
-      <c r="O61">
+      <c r="O60">
         <f t="shared" si="17"/>
         <v>1</v>
       </c>
-      <c r="P61">
+      <c r="P60">
         <f t="shared" si="18"/>
         <v>1</v>
       </c>
-      <c r="R61">
+      <c r="R60">
         <f t="shared" si="19"/>
         <v>10</v>
       </c>
-      <c r="T61">
-        <v>10</v>
+      <c r="T60">
+        <v>0</v>
       </c>
     </row>
     <row r="62" spans="1:20">
       <c r="A62" t="s">
-        <v>87</v>
+        <v>48</v>
       </c>
       <c r="B62">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="C62">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D62" t="s">
-        <v>51</v>
+        <v>50</v>
+      </c>
+      <c r="G62" t="s">
+        <v>86</v>
       </c>
       <c r="N62">
         <f t="shared" si="16"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O62">
         <f t="shared" si="17"/>
@@ -1861,55 +1854,52 @@
     </row>
     <row r="63" spans="1:20">
       <c r="A63" t="s">
-        <v>52</v>
+        <v>85</v>
       </c>
       <c r="B63">
-        <v>100</v>
+        <v>40</v>
       </c>
       <c r="C63">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="D63" t="s">
-        <v>51</v>
-      </c>
-      <c r="G63" t="s">
-        <v>72</v>
+        <v>50</v>
       </c>
       <c r="N63">
         <f t="shared" si="16"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="O63">
         <f t="shared" si="17"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="P63">
         <f t="shared" si="18"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R63">
         <f t="shared" si="19"/>
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="T63">
-        <v>20</v>
+        <v>10</v>
       </c>
     </row>
     <row r="64" spans="1:20">
       <c r="A64" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="B64">
         <v>100</v>
       </c>
       <c r="C64">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="D64" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G64" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="N64">
         <f t="shared" si="16"/>
@@ -1933,55 +1923,55 @@
     </row>
     <row r="65" spans="1:20">
       <c r="A65" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B65">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="C65">
         <v>30</v>
       </c>
       <c r="D65" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G65" t="s">
-        <v>89</v>
+        <v>71</v>
       </c>
       <c r="N65">
         <f t="shared" si="16"/>
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="O65">
         <f t="shared" si="17"/>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="P65">
         <f t="shared" si="18"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="R65">
         <f t="shared" si="19"/>
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="T65">
-        <v>30</v>
+        <v>20</v>
       </c>
     </row>
     <row r="66" spans="1:20">
       <c r="A66" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B66">
         <v>200</v>
       </c>
       <c r="C66">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D66" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="G66" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="N66">
         <f t="shared" si="16"/>
@@ -2003,82 +1993,113 @@
         <v>30</v>
       </c>
     </row>
-    <row r="68" spans="1:20">
-      <c r="A68" t="s">
-        <v>92</v>
-      </c>
-      <c r="B68">
+    <row r="67" spans="1:20">
+      <c r="A67" t="s">
+        <v>53</v>
+      </c>
+      <c r="B67">
+        <v>200</v>
+      </c>
+      <c r="C67">
+        <v>35</v>
+      </c>
+      <c r="D67" t="s">
+        <v>54</v>
+      </c>
+      <c r="G67" t="s">
+        <v>88</v>
+      </c>
+      <c r="N67">
+        <f t="shared" si="16"/>
+        <v>10</v>
+      </c>
+      <c r="O67">
+        <f t="shared" si="17"/>
+        <v>5</v>
+      </c>
+      <c r="P67">
+        <f t="shared" si="18"/>
+        <v>4</v>
+      </c>
+      <c r="R67">
+        <f t="shared" si="19"/>
+        <v>40</v>
+      </c>
+      <c r="T67">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="69" spans="1:20">
+      <c r="A69" t="s">
+        <v>90</v>
+      </c>
+      <c r="B69">
         <v>100</v>
       </c>
-      <c r="C68">
+      <c r="C69">
         <v>20</v>
       </c>
-      <c r="D68" t="s">
-        <v>57</v>
-      </c>
-      <c r="N68">
-        <f t="shared" ref="N67:N70" si="20">CEILING(B68/$B$32,1)</f>
+      <c r="D69" t="s">
+        <v>56</v>
+      </c>
+      <c r="N69">
+        <f t="shared" ref="N69:N71" si="20">CEILING(B69/$B$32,1)</f>
         <v>5</v>
       </c>
-      <c r="O68">
-        <f t="shared" ref="O67:O70" si="21">CEILING(B68/$B$33,1)</f>
+      <c r="O69">
+        <f t="shared" ref="O69:O71" si="21">CEILING(B69/$B$33,1)</f>
         <v>3</v>
       </c>
-      <c r="P68">
-        <f t="shared" ref="P67:P70" si="22">CEILING(B68/$B$34,1)</f>
+      <c r="P69">
+        <f t="shared" ref="P69:P71" si="22">CEILING(B69/$B$34,1)</f>
         <v>2</v>
       </c>
-      <c r="R68">
+      <c r="R69">
         <f t="shared" si="19"/>
         <v>20</v>
       </c>
-      <c r="T68">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="70" spans="1:20">
-      <c r="A70" t="s">
-        <v>91</v>
-      </c>
-      <c r="B70">
+      <c r="T69">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="71" spans="1:20">
+      <c r="A71" t="s">
+        <v>89</v>
+      </c>
+      <c r="B71">
         <v>300</v>
       </c>
-      <c r="C70">
+      <c r="C71">
         <v>30</v>
       </c>
-      <c r="N70">
+      <c r="N71">
         <f t="shared" si="20"/>
         <v>15</v>
       </c>
-      <c r="O70">
+      <c r="O71">
         <f t="shared" si="21"/>
         <v>8</v>
       </c>
-      <c r="P70">
+      <c r="P71">
         <f t="shared" si="22"/>
         <v>5</v>
       </c>
-      <c r="R70">
+      <c r="R71">
         <f t="shared" si="19"/>
         <v>50</v>
       </c>
-      <c r="T70">
+      <c r="T71">
         <v>30</v>
       </c>
     </row>
-    <row r="73" spans="1:20">
-      <c r="A73" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="75" spans="1:20">
-      <c r="A75" t="s">
-        <v>67</v>
+    <row r="74" spans="1:20">
+      <c r="A74" s="1" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="76" spans="1:20">
       <c r="A76" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="77" spans="1:20">
@@ -2088,22 +2109,27 @@
     </row>
     <row r="78" spans="1:20">
       <c r="A78" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
     </row>
     <row r="79" spans="1:20">
       <c r="A79" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="80" spans="1:20">
       <c r="A80" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="81" spans="1:1">
       <c r="A81" t="s">
-        <v>66</v>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1">
+      <c r="A82" t="s">
+        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>